<commit_message>
Today's updates (27th July)
</commit_message>
<xml_diff>
--- a/OSC_demographics_updated.xlsx
+++ b/OSC_demographics_updated.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\York University\LabYU\HH Visual and Cognitive Development Project\OSC-Study\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\York University\LabYU\HH Visual and Cognitive Development Project\OSC-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2561,7 +2561,7 @@
   <dimension ref="A1:AF1019"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q205" sqref="Q205"/>
     </sheetView>
   </sheetViews>

</xml_diff>